<commit_message>
Update CA Excel files with latest revisions
</commit_message>
<xml_diff>
--- a/BTS101.CA.xlsx
+++ b/BTS101.CA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\CA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08EEC873-5DC9-42A2-8B65-042CC8D15754}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5068DC15-B6FE-4F91-9979-E3EAFCE1784B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -581,7 +581,7 @@
   <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -686,7 +686,7 @@
         <v>15</v>
       </c>
       <c r="D4" s="1">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E4" s="2">
         <v>10.03125</v>
@@ -868,7 +868,7 @@
         <v>15</v>
       </c>
       <c r="D11" s="1">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E11" s="2">
         <v>9.59375</v>
@@ -894,7 +894,7 @@
         <v>15</v>
       </c>
       <c r="D12" s="1">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E12" s="2">
         <v>12.71875</v>

</xml_diff>